<commit_message>
move design and logo to document folder
</commit_message>
<xml_diff>
--- a/documents/API List.xlsx
+++ b/documents/API List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.Work\Graduate\front\SESTOPIA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489903D1-778B-470F-84C2-2C81FB07D665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04F35F9-9A9E-488F-8ABC-792CDC5CFA98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
optimaze the search api
</commit_message>
<xml_diff>
--- a/documents/API List.xlsx
+++ b/documents/API List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.Work\Graduate\front\SESTOPIA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04F35F9-9A9E-488F-8ABC-792CDC5CFA98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2FE919-FEAE-4AB3-94A7-573B024E6674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,6 +153,42 @@
   </si>
   <si>
     <t>/api/skills/search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    {
+        "id": 1, 
+        "name": "API Implementation", 
+        "classification": "", 
+        "prerequisites": null, 
+        "knowledge_area": "Software Construction", 
+        "rationale": null, 
+        "roles_for_skill": null, 
+        "related_activities": null, 
+        "real_world_scenario": null, 
+        "role_of_academia": null, 
+        "tools": null, 
+        "self_assessment": null, 
+        "reference": null, 
+        "student_name": "Baiyu Huo", 
+        "student_no": 40076004
+    }, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/skills/{member id}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -552,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -666,12 +702,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+    <row r="6" spans="1:7" ht="234.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="5"/>
     </row>

</xml_diff>